<commit_message>
fix assign role & check his accuracy
</commit_message>
<xml_diff>
--- a/src/audio_and_experiment/structured_data_manual.xlsx
+++ b/src/audio_and_experiment/structured_data_manual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Meditation-Interviews\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Meditation-Interviews\src\audio_and_experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C830962-C23F-44F4-B3EE-74D65B045485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C321F772-DA90-4940-92D8-9FFEE1D714D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D7D4240-F1F1-462A-A574-7C1F6EBCACE7}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="97">
   <si>
     <t>Experiment</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>S313</t>
+  </si>
+  <si>
+    <t>Moslty empty</t>
   </si>
 </sst>
 </file>
@@ -1200,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC2A6DB-C6FD-412D-9D85-CA9107A99F38}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1768,7 +1771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1788,7 +1791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1808,7 +1811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1868,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -1928,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1948,7 +1951,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -1988,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -2008,7 +2011,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -2064,11 +2067,14 @@
       <c r="E47" t="s">
         <v>33</v>
       </c>
-      <c r="F47" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -2206,6 +2212,9 @@
       </c>
       <c r="F54" t="s">
         <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2775,7 +2784,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F82">
+  <conditionalFormatting sqref="F1:F82 G44 G47 G54">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2790,5 +2799,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>